<commit_message>
Grid added for paraller run
</commit_message>
<xml_diff>
--- a/PageObjectModel/Data/Data.xlsx
+++ b/PageObjectModel/Data/Data.xlsx
@@ -11,12 +11,12 @@
     <sheet name="TestData" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Runmode</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Subitems</t>
+  </si>
+  <si>
+    <t>SelectProduct</t>
+  </si>
+  <si>
+    <t>Printed Dress</t>
   </si>
 </sst>
 </file>
@@ -522,7 +528,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,6 +612,9 @@
       <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -613,6 +622,9 @@
       </c>
       <c r="B8" t="s">
         <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>